<commit_message>
Update last working version for meeting
</commit_message>
<xml_diff>
--- a/control_panel.xlsx
+++ b/control_panel.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Projects\VUPEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978D0EF2-4AD2-461C-9AFD-645C657DDFE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3E6581-C6D4-4EEE-87D4-2BD46A2977C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" xr2:uid="{59D61454-8C61-4688-B56E-9C111FDC046B}"/>
+    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" activeTab="1" xr2:uid="{59D61454-8C61-4688-B56E-9C111FDC046B}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
-    <sheet name="Physical" sheetId="2" r:id="rId2"/>
-    <sheet name="Accessories" sheetId="5" r:id="rId3"/>
-    <sheet name="Drivetrain" sheetId="3" r:id="rId4"/>
-    <sheet name="Motors" sheetId="7" r:id="rId5"/>
-    <sheet name="Battery" sheetId="8" r:id="rId6"/>
+    <sheet name="Vehicle" sheetId="10" r:id="rId2"/>
+    <sheet name="Environment" sheetId="2" r:id="rId3"/>
+    <sheet name="Accessories" sheetId="5" r:id="rId4"/>
+    <sheet name="Drivetrain" sheetId="3" r:id="rId5"/>
+    <sheet name="Motors" sheetId="7" r:id="rId6"/>
+    <sheet name="Battery" sheetId="8" r:id="rId7"/>
+    <sheet name="donttouch" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
   <si>
     <t>Parameter</t>
   </si>
@@ -50,9 +52,6 @@
     <t>preset_manufacturer</t>
   </si>
   <si>
-    <t>this value must exist in /data/drivecycles as a named cycle</t>
-  </si>
-  <si>
     <t>mass</t>
   </si>
   <si>
@@ -65,39 +64,18 @@
     <t>Notes on behaviour</t>
   </si>
   <si>
-    <t>default: default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If set, will lookup manufacturer : vehicle.  </t>
-  </si>
-  <si>
     <t>Notes on values</t>
   </si>
   <si>
-    <t>can be sedan, coupe, etc. or an actual model</t>
-  </si>
-  <si>
     <t>blank, or mass in kg</t>
   </si>
   <si>
     <t>default: fwd</t>
   </si>
   <si>
-    <t>formal_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if true, uses the actual test parameters, e.g. no accessories, perfect driving, etc. </t>
-  </si>
-  <si>
-    <t>true (default), false</t>
-  </si>
-  <si>
     <t>would like to have this actually linked to the db, but not much chance</t>
   </si>
   <si>
-    <t>e.g. 2020</t>
-  </si>
-  <si>
     <t>Don't use this at present</t>
   </si>
   <si>
@@ -113,15 +91,9 @@
     <t>default: all season,  winter, offroad, sports</t>
   </si>
   <si>
-    <t>default: nedc</t>
-  </si>
-  <si>
     <t>Physical Parameters and Conditions</t>
   </si>
   <si>
-    <t>Vehicle Extended</t>
-  </si>
-  <si>
     <t>Vehicle Setup</t>
   </si>
   <si>
@@ -372,13 +344,89 @@
   </si>
   <si>
     <t>e.g. 96</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>sedan</t>
+  </si>
+  <si>
+    <t>coupe</t>
+  </si>
+  <si>
+    <t>suv</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>compact</t>
+  </si>
+  <si>
+    <t>bev</t>
+  </si>
+  <si>
+    <t>nedc</t>
+  </si>
+  <si>
+    <t>eudc</t>
+  </si>
+  <si>
+    <t>hwfe</t>
+  </si>
+  <si>
+    <t>ftp</t>
+  </si>
+  <si>
+    <t>wltp 3a</t>
+  </si>
+  <si>
+    <t>wltp 3b</t>
+  </si>
+  <si>
+    <t>wltp 2</t>
+  </si>
+  <si>
+    <t>wltp 1</t>
+  </si>
+  <si>
+    <t>These options form the base of the vehicle parameters and will fill in all values with defaults where not otherwise specified</t>
+  </si>
+  <si>
+    <t>tire_size</t>
+  </si>
+  <si>
+    <t>Vehicle Parameters</t>
+  </si>
+  <si>
+    <t>This will also set the default environment parameters, e.g. temperature.</t>
+  </si>
+  <si>
+    <t>If any of these are set, results may not represent the formal test parameters for the drive cycle</t>
+  </si>
+  <si>
+    <t>Calculation Mode</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>A/B</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>In A/B mode, the vehicle specified with entered values will be compared to that of the base vehicle determined on this page.   
+In Sensitivity mode, any entered parameters will be taken as the base vehicle, and a sensitivity analysis will be performed for all numeric parameters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +473,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +526,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -663,6 +747,50 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,6 +806,259 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E11" fmlaRange="donttouch!$B$1:$B$1" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E12" fmlaRange="donttouch!$C$1:$C$6" noThreeD="1" sel="3" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E16" fmlaRange="donttouch!$D$1:$D$8" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E8" fmlaRange="donttouch!$A$1:$A$2" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>68580</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>22860</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>274320</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>53340</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>22860</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>259080</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Drop Down 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E569B5-27CE-4326-A583-48EDFF45642F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>7620</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>45720</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>251460</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Drop Down 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632BD6D1-9868-41F0-AD66-1CE8C9CFE692}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>1356360</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>182880</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>15240</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>388620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Drop Down 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3AA2A4-3AEE-4F3A-9466-30B3FA201BF6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -976,11 +1357,365 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA88FBD-B2AC-4A2D-8C28-2F8E0733F205}">
-  <dimension ref="B1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA88FBD-B2AC-4A2D-8C28-2F8E0733F205}">
+  <dimension ref="B1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="2:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="2:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="2:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="45">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
+      <c r="C11" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
+      <c r="E11" s="45">
+        <v>1</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="45">
+        <v>3</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="34">
+        <v>2020</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="33">
+        <v>1</v>
+      </c>
+      <c r="E16" s="45">
+        <v>1</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="15"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId4" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>68580</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>274320</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId5" name="Drop Down 3">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>53340</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>259080</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2052" r:id="rId6" name="Drop Down 4">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>45720</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>30480</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>251460</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId7" name="Drop Down 6">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>1356360</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>182880</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>388620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5B868B-F875-4A5D-A4C3-8FEC2C356BDD}">
+  <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1735,7 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1028,11 +1763,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1046,249 +1781,206 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="19"/>
+      <c r="C7" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="36"/>
       <c r="E7" s="8"/>
       <c r="F7" s="23" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="19"/>
+      <c r="C8" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="36"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="19"/>
+      <c r="C9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="36"/>
       <c r="E9" s="8"/>
       <c r="F9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="13"/>
+      <c r="C10" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
+      <c r="C11" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
-      <c r="C12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="19"/>
+      <c r="C12" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="36"/>
       <c r="E12" s="8"/>
       <c r="F12" s="23" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
-      <c r="C13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="19"/>
+      <c r="C13" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="36"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="23" t="s">
-        <v>16</v>
+      <c r="F13" s="31" t="s">
+        <v>49</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="19"/>
+      <c r="C14" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="36"/>
       <c r="E14" s="8"/>
       <c r="F14" s="23" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="21"/>
+      <c r="H14" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="21"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-      <c r="C17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" s="1" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="2:7" s="1" customFormat="1" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AA93F9-9C0A-4254-8FB7-D1649D3E71D2}">
-  <dimension ref="B1:H24"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,14 +2000,16 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="16"/>
+      <c r="H2" s="40" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
@@ -1336,11 +2030,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1353,213 +2047,142 @@
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="6"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="31" t="s">
-        <v>59</v>
+      <c r="F9" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
       <c r="F10" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="21"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="15"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="3:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="3:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="3:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39371A6-40C3-42FE-9D8A-70D3EEE03244}">
   <dimension ref="B1:H21"/>
   <sheetViews>
@@ -1584,7 +2207,7 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1612,11 +2235,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1630,7 +2253,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -1642,12 +2265,12 @@
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="8"/>
       <c r="F7" s="23" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="21"/>
@@ -1655,42 +2278,42 @@
     <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="8"/>
       <c r="F9" s="23" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
       <c r="F10" s="23" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="21"/>
@@ -1698,7 +2321,7 @@
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="8"/>
@@ -1709,16 +2332,16 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="8"/>
       <c r="F12" s="23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="21" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
@@ -1792,7 +2415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B7035C-9660-4135-8D23-9C07094EBB0E}">
   <dimension ref="B1:H20"/>
   <sheetViews>
@@ -1817,7 +2440,7 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1845,11 +2468,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1863,7 +2486,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -1875,27 +2498,27 @@
     <row r="7" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="8"/>
       <c r="F7" s="23" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="21" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="21"/>
@@ -1903,12 +2526,12 @@
     <row r="9" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="8"/>
       <c r="F9" s="23" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="21"/>
@@ -1916,16 +2539,16 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
       <c r="F10" s="23" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -2008,7 +2631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE3A771-BFF8-4509-8841-4D696BBB30F7}">
   <dimension ref="B1:H26"/>
   <sheetViews>
@@ -2033,7 +2656,7 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2061,11 +2684,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2079,7 +2702,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -2091,12 +2714,12 @@
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="8"/>
       <c r="F7" s="23" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="21"/>
@@ -2104,12 +2727,12 @@
     <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="21"/>
@@ -2117,25 +2740,25 @@
     <row r="9" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="7" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="8"/>
       <c r="F9" s="23"/>
       <c r="G9" s="8"/>
       <c r="H9" s="21" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
       <c r="F10" s="23" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="21"/>
@@ -2143,12 +2766,12 @@
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="8"/>
       <c r="F11" s="23" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="21"/>
@@ -2164,7 +2787,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
@@ -2176,12 +2799,12 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="8"/>
       <c r="F14" s="23" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="21"/>
@@ -2189,12 +2812,12 @@
     <row r="15" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="8"/>
       <c r="F15" s="23" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="21"/>
@@ -2202,12 +2825,12 @@
     <row r="16" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="8"/>
       <c r="F16" s="23" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="21"/>
@@ -2215,14 +2838,14 @@
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
       <c r="C17" s="7" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="8"/>
       <c r="F17" s="23"/>
       <c r="G17" s="8"/>
       <c r="H17" s="21" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -2296,7 +2919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2418CB-A920-4DCA-80E8-6BD088A3B5D0}">
   <dimension ref="B1:H27"/>
   <sheetViews>
@@ -2321,7 +2944,7 @@
     <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2349,11 +2972,11 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2367,7 +2990,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -2379,12 +3002,12 @@
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="8"/>
       <c r="F7" s="23" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="21"/>
@@ -2392,12 +3015,12 @@
     <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
       <c r="F8" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="21"/>
@@ -2413,7 +3036,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
@@ -2425,12 +3048,12 @@
     <row r="11" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="8"/>
       <c r="F11" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="21"/>
@@ -2438,12 +3061,12 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="8"/>
       <c r="F12" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="20"/>
@@ -2451,12 +3074,12 @@
     <row r="13" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="8"/>
       <c r="F13" s="23" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="21"/>
@@ -2472,7 +3095,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
@@ -2484,12 +3107,12 @@
     <row r="16" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="8"/>
       <c r="F16" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="21"/>
@@ -2497,12 +3120,12 @@
     <row r="17" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
       <c r="C17" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="8"/>
       <c r="F17" s="23" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="21"/>
@@ -2510,12 +3133,12 @@
     <row r="18" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14"/>
       <c r="C18" s="7" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="8"/>
       <c r="F18" s="23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="21"/>
@@ -2589,4 +3212,198 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FB9EE0-658B-44D0-A212-7083A1650233}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big update for showtime
</commit_message>
<xml_diff>
--- a/control_panel.xlsx
+++ b/control_panel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Projects\VUPEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3E6581-C6D4-4EEE-87D4-2BD46A2977C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE67ACB9-C0CB-443A-9818-D7A3EFCF0F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" activeTab="1" xr2:uid="{59D61454-8C61-4688-B56E-9C111FDC046B}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
     <sheet name="Vehicle" sheetId="10" r:id="rId2"/>
     <sheet name="Environment" sheetId="2" r:id="rId3"/>
-    <sheet name="Accessories" sheetId="5" r:id="rId4"/>
-    <sheet name="Drivetrain" sheetId="3" r:id="rId5"/>
-    <sheet name="Motors" sheetId="7" r:id="rId6"/>
-    <sheet name="Battery" sheetId="8" r:id="rId7"/>
+    <sheet name="Battery" sheetId="8" r:id="rId4"/>
+    <sheet name="Accessories" sheetId="5" r:id="rId5"/>
+    <sheet name="Drivetrain" sheetId="3" r:id="rId6"/>
+    <sheet name="Motors" sheetId="7" r:id="rId7"/>
     <sheet name="donttouch" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -813,15 +813,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E12" fmlaRange="donttouch!$C$1:$C$6" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E12" fmlaRange="donttouch!$C$1:$C$6" noThreeD="1" sel="4" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E16" fmlaRange="donttouch!$D$1:$D$8" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E16" fmlaRange="donttouch!$D$1:$D$8" noThreeD="1" sel="3" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E8" fmlaRange="donttouch!$A$1:$A$2" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="E8" fmlaRange="donttouch!$A$1:$A$2" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,7 +907,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E569B5-27CE-4326-A583-48EDFF45642F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -965,7 +965,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632BD6D1-9868-41F0-AD66-1CE8C9CFE692}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1023,7 +1023,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3AA2A4-3AEE-4F3A-9466-30B3FA201BF6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1361,7 +1361,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="D8" s="42"/>
       <c r="E8" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="41" t="s">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="38" t="s">
@@ -1539,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="38" t="s">
@@ -1715,7 +1715,7 @@
   <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,7 +1930,6 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1980,7 +1979,7 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2183,11 +2182,306 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2418CB-A920-4DCA-80E8-6BD088A3B5D0}">
+  <dimension ref="B1:H27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" activeCellId="1" sqref="H16 C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="57" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
+      <c r="C8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="14"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
+      <c r="C11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14"/>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="14"/>
+      <c r="C18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="15"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="2:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39371A6-40C3-42FE-9D8A-70D3EEE03244}">
   <dimension ref="B1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D29"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2415,12 +2709,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B7035C-9660-4135-8D23-9C07094EBB0E}">
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2631,7 +2925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE3A771-BFF8-4509-8841-4D696BBB30F7}">
   <dimension ref="B1:H26"/>
   <sheetViews>
@@ -2919,307 +3213,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2418CB-A920-4DCA-80E8-6BD088A3B5D0}">
-  <dimension ref="B1:H27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" activeCellId="1" sqref="H16 C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="57" style="2" customWidth="1"/>
-    <col min="9" max="9" width="2" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="21"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="2:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="2:8" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="2:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-      <c r="C17" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FB9EE0-658B-44D0-A212-7083A1650233}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>